<commit_message>
update plan test + MAJ  méthod load et save pour local storage
</commit_message>
<xml_diff>
--- a/frontend/mapping/plan_tests.xlsx
+++ b/frontend/mapping/plan_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\GitHub\p5\frontend\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71014F6-5B8E-4A18-96B0-EDA2CDF028FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC33B9F4-301B-4460-B057-804BE13D6CAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16CB7D35-3DD2-412C-9FEC-88DEC5ED953D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>Résultat à obtenir</t>
   </si>
@@ -77,12 +77,6 @@
     <t>oui</t>
   </si>
   <si>
-    <t>non</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>addProductToCart</t>
   </si>
   <si>
@@ -147,13 +141,43 @@
   </si>
   <si>
     <t>En passant un produit, on s'assure de récupérer les caractéristiques du produit sélectionné par l'utilisateur : création des div dédiées</t>
+  </si>
+  <si>
+    <t>L'appel de cette fonction doit simplement retourner un message d'erreur si le panier est vide</t>
+  </si>
+  <si>
+    <t>En ajoutant une item au panier, on s'assure que l'appel de cette méthode vide correctement le local storage</t>
+  </si>
+  <si>
+    <t>En ajoutant une item au panier, on s'assure que l'appel de cette méthode ajoute correctement l'item au local storage dédié au badge (nécessite ensuite l'appel de la méthode refreshBadge())</t>
+  </si>
+  <si>
+    <t>En ajoutant une item au panier, on s'assure que le refresh du badge s'opère après l'update de celui-ci dans le local storage (cf. updateBadge())</t>
+  </si>
+  <si>
+    <t>En saisissant un des champs disponibles dans le formulaire, on s'assure que l'utilisateur respecte le format attendu concernant les informations saisies</t>
+  </si>
+  <si>
+    <t>En appelant cette méthode, on s'assur de récupérer la couleur et la quantité choisie par l'utilisateur (value)</t>
+  </si>
+  <si>
+    <t>saveLocalStorage</t>
+  </si>
+  <si>
+    <t>loadLocalStorage</t>
+  </si>
+  <si>
+    <t>En passant une id, on s'assure qu'on obtient bien ce qui est disponible dans le local storage</t>
+  </si>
+  <si>
+    <t>En passant une id et une value, on s'assure d'effectuer une sauvegarde conforme dans le local storage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,59 +187,67 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color rgb="FF0070C0"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <sz val="10"/>
+      <color rgb="FFFF0066"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
       <i/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0066"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -244,16 +276,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -262,13 +289,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -277,9 +304,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,19 +632,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19773466-3432-496F-B485-06B9F9E3B71C}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="75.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="75.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.140625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -625,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -639,7 +673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -653,11 +687,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -667,7 +701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -678,82 +712,82 @@
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
+      <c r="B7" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
+      <c r="B8" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>5</v>
@@ -762,282 +796,311 @@
         <v>12</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="4" t="s">
+    <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="4" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="C15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="9"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="14"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="7"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="7"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="10"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="14"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="14"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="14"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
     </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{2028D164-5DCA-489E-BD88-0CE41A75978E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Responsive + Design
</commit_message>
<xml_diff>
--- a/frontend/mapping/plan_tests.xlsx
+++ b/frontend/mapping/plan_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\GitHub\p5\frontend\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC33B9F4-301B-4460-B057-804BE13D6CAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A07094-CC9A-4181-8739-40206F73B2ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16CB7D35-3DD2-412C-9FEC-88DEC5ED953D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>Résultat à obtenir</t>
   </si>
@@ -60,12 +60,6 @@
   </si>
   <si>
     <t>product.js</t>
-  </si>
-  <si>
-    <t>ajaxGet</t>
-  </si>
-  <si>
-    <t>En passant un produit, on s'assure de récupérer, via l'id disponible dans l'url de la page, le produit sélectionné par l'utilisateur</t>
   </si>
   <si>
     <t>Fonctions</t>
@@ -632,7 +626,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19773466-3432-496F-B485-06B9F9E3B71C}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -650,10 +644,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -667,7 +661,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>4</v>
@@ -681,55 +675,55 @@
         <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>8</v>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>5</v>
+      <c r="B5" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -737,196 +731,188 @@
         <v>13</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="6" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>38</v>
+        <v>10</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="6"/>
     </row>
@@ -1045,16 +1031,16 @@
       <c r="D41" s="6"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
-      <c r="D42" s="6"/>
+      <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="11"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="14"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
@@ -1064,15 +1050,15 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
       <c r="D45" s="14"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
-      <c r="D46" s="14"/>
+      <c r="D46" s="12"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
@@ -1091,12 +1077,6 @@
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{2028D164-5DCA-489E-BD88-0CE41A75978E}"/>

</xml_diff>